<commit_message>
Additional columns added to date M query
Still in draft
</commit_message>
<xml_diff>
--- a/date_table.xlsx
+++ b/date_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin.corbin\Documents\GitHub\wa-date-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6A8F6E-7EA3-4346-AECE-6061CEF4E1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620EC9BD-58C3-49A1-96FA-A21EDA792985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="255" windowWidth="25800" windowHeight="15495" xr2:uid="{E8A0502C-8DE7-45E0-8320-080B1C53CC6E}"/>
   </bookViews>
@@ -167,12 +167,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>year_quarter</t>
-  </si>
-  <si>
-    <t>year_month</t>
-  </si>
-  <si>
     <t>month_end_flag</t>
   </si>
   <si>
@@ -258,6 +252,12 @@
   </si>
   <si>
     <t>cy_month_number_overall</t>
+  </si>
+  <si>
+    <t>cal_year_quarter</t>
+  </si>
+  <si>
+    <t>cal_year_month</t>
   </si>
 </sst>
 </file>
@@ -341,10 +341,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,7 +643,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -691,13 +687,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -729,7 +725,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -757,7 +753,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -767,15 +763,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,118 +796,118 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draft date table complete
Added draft fields to date table. There are errors which need fixes
</commit_message>
<xml_diff>
--- a/date_table.xlsx
+++ b/date_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin.corbin\Documents\GitHub\wa-date-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620EC9BD-58C3-49A1-96FA-A21EDA792985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EE44AA-BB50-4627-8780-65AD9D8267FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="255" windowWidth="25800" windowHeight="15495" xr2:uid="{E8A0502C-8DE7-45E0-8320-080B1C53CC6E}"/>
   </bookViews>
@@ -88,36 +88,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{BBD08D8C-5BDE-40E3-9798-DBBA1829F055}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Colin Corbin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Either 1 or 2 for biennium year one or biennium yr 2</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>date_key</t>
   </si>
@@ -188,15 +164,6 @@
     <t>YYYY</t>
   </si>
   <si>
-    <t>biennium_yr_1</t>
-  </si>
-  <si>
-    <t>biennium_yr_2</t>
-  </si>
-  <si>
-    <t>fy_index</t>
-  </si>
-  <si>
     <t>fiscal_year</t>
   </si>
   <si>
@@ -206,24 +173,12 @@
     <t>week_num_in_fy</t>
   </si>
   <si>
-    <t>day_num_in_fm</t>
-  </si>
-  <si>
     <t>day_num_in_fy</t>
   </si>
   <si>
-    <t>week_num_in_biennium</t>
-  </si>
-  <si>
     <t>day_num_in_biennium</t>
   </si>
   <si>
-    <t>month_num_in_fy</t>
-  </si>
-  <si>
-    <t>month_num_in_biennium</t>
-  </si>
-  <si>
     <t>fiscal_quarter</t>
   </si>
   <si>
@@ -258,6 +213,12 @@
   </si>
   <si>
     <t>cal_year_month</t>
+  </si>
+  <si>
+    <t>biennium_yr</t>
+  </si>
+  <si>
+    <t>1 or 2</t>
   </si>
 </sst>
 </file>
@@ -640,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C4F115-F91B-499C-AEFA-27A98E0D9A38}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -687,13 +648,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -725,7 +686,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -753,7 +714,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -763,15 +724,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -796,12 +757,12 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -839,75 +800,48 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Date table DDL updates and bug fixes
Updated column names to make them consistent. Bug fix on M query function
</commit_message>
<xml_diff>
--- a/date_table.xlsx
+++ b/date_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin.corbin\Documents\GitHub\wa-date-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EE44AA-BB50-4627-8780-65AD9D8267FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28797969-7171-47B4-8AC6-C3E3C45805A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="255" windowWidth="25800" windowHeight="15495" xr2:uid="{E8A0502C-8DE7-45E0-8320-080B1C53CC6E}"/>
+    <workbookView xWindow="18810" yWindow="1125" windowWidth="7380" windowHeight="15495" xr2:uid="{E8A0502C-8DE7-45E0-8320-080B1C53CC6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{0C883B64-6175-4E93-BB3A-C578F7AC7392}">
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{0C883B64-6175-4E93-BB3A-C578F7AC7392}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>date_key</t>
   </si>
@@ -122,12 +122,6 @@
     <t>weekday_flag</t>
   </si>
   <si>
-    <t>week_num_in_yr</t>
-  </si>
-  <si>
-    <t>week_num_overall</t>
-  </si>
-  <si>
     <t>week_begin_date</t>
   </si>
   <si>
@@ -137,12 +131,6 @@
     <t>month_abbrev</t>
   </si>
   <si>
-    <t>quarter</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>month_end_flag</t>
   </si>
   <si>
@@ -167,24 +155,9 @@
     <t>fiscal_year</t>
   </si>
   <si>
-    <t>fiscal_month</t>
-  </si>
-  <si>
-    <t>week_num_in_fy</t>
-  </si>
-  <si>
-    <t>day_num_in_fy</t>
-  </si>
-  <si>
-    <t>day_num_in_biennium</t>
-  </si>
-  <si>
     <t>fiscal_quarter</t>
   </si>
   <si>
-    <t>fiscal_year_quarte</t>
-  </si>
-  <si>
     <t>YYQQ</t>
   </si>
   <si>
@@ -197,28 +170,79 @@
     <t>Example</t>
   </si>
   <si>
-    <t>overall_day_nbr</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
-    <t>cy_month_number</t>
-  </si>
-  <si>
-    <t>cy_month_number_overall</t>
-  </si>
-  <si>
-    <t>cal_year_quarter</t>
-  </si>
-  <si>
-    <t>cal_year_month</t>
-  </si>
-  <si>
-    <t>biennium_yr</t>
-  </si>
-  <si>
     <t>1 or 2</t>
+  </si>
+  <si>
+    <t>calendar_quarter</t>
+  </si>
+  <si>
+    <t>calendar_year</t>
+  </si>
+  <si>
+    <t>calendar_year_month_number</t>
+  </si>
+  <si>
+    <t>calendar_year_month_number_overall</t>
+  </si>
+  <si>
+    <t>calendar_year_quarter</t>
+  </si>
+  <si>
+    <t>fiscal_year_quarter</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>smallint not null</t>
+  </si>
+  <si>
+    <t>smalldatetime</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>varchar(9)</t>
+  </si>
+  <si>
+    <t>varchar(3)</t>
+  </si>
+  <si>
+    <t>char(1)</t>
+  </si>
+  <si>
+    <t>week_begin_date_key</t>
+  </si>
+  <si>
+    <t>fiscal_month_number</t>
+  </si>
+  <si>
+    <t>week_number_overall</t>
+  </si>
+  <si>
+    <t>day_number_overall</t>
+  </si>
+  <si>
+    <t>week_number_in_calendar_year</t>
+  </si>
+  <si>
+    <t>biennium_year</t>
+  </si>
+  <si>
+    <t>fiscal_year_day_number</t>
+  </si>
+  <si>
+    <t>fiscal_year_week_number</t>
+  </si>
+  <si>
+    <t>biennium_day_number</t>
   </si>
 </sst>
 </file>
@@ -255,12 +279,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -284,9 +314,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,247 +632,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C4F115-F91B-499C-AEFA-27A98E0D9A38}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>20130101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
         <v>21</v>
       </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>